<commit_message>
update statistics by excel
</commit_message>
<xml_diff>
--- a/myfundStatistics.xlsx
+++ b/myfundStatistics.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testGit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1705DB4F-A01B-4F6C-820E-354E5B655EDE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12765" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" calcMode="manual" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>日期</t>
   </si>
@@ -224,32 +230,43 @@
   </si>
   <si>
     <t>0.9328</t>
+  </si>
+  <si>
+    <t>sadsad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asdasdsad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -265,15 +282,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -539,23 +565,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="13.375"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -595,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -615,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -635,7 +657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -655,7 +677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -675,7 +697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -695,7 +717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -715,7 +737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -735,7 +757,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -755,7 +777,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -775,7 +797,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -795,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -815,7 +837,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -835,7 +857,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -855,7 +877,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -875,7 +897,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -895,7 +917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -915,8 +937,22 @@
         <v>41</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>